<commit_message>
test cases for single value & list<String>
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,9 +20,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n12</t>
   </si>
 </sst>
 </file>
@@ -33,7 +72,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -54,6 +93,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,12 +142,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -124,10 +172,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -147,11 +195,66 @@
       <c r="C1" s="0" t="n">
         <v>1.3</v>
       </c>
-      <c r="D1" s="0" t="n">
+      <c r="D1" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="b">
-        <v>1</v>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more tests / mainly for List
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -72,7 +72,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,11 +93,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,7 +146,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,10 +167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -257,6 +252,296 @@
         <v>13</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
enum support & test for List<UserObject>
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -62,6 +62,45 @@
   </si>
   <si>
     <t xml:space="preserve">n12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiliams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
   </si>
 </sst>
 </file>
@@ -167,10 +206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,6 +291,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1</v>
@@ -369,89 +413,116 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="b">
+      <c r="A17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="b">
+      <c r="A18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="b">
+      <c r="A19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -540,6 +611,62 @@
       </c>
       <c r="I24" s="0" t="n">
         <v>3.7</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
default behavior for value cell in Map & more tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -206,10 +206,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -413,89 +413,116 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="b">
+      <c r="A17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="b">
+      <c r="A18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="b">
+      <c r="A19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -639,6 +666,71 @@
         <v>23</v>
       </c>
       <c r="D30" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more tests & handled when iterating over columns as FIXED
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -101,6 +101,27 @@
   </si>
   <si>
     <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dmytro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimon.mula</t>
   </si>
 </sst>
 </file>
@@ -206,17 +227,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,6 +755,154 @@
       </c>
       <c r="E35" s="0" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>89123123</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>89123123</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>89123123</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved a few places & more test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t xml:space="preserve">dimon.mula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etc</t>
   </si>
 </sst>
 </file>
@@ -227,10 +230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -905,6 +908,168 @@
         <v>33</v>
       </c>
     </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
validation for user inputs & exceptions
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -125,6 +125,93 @@
   </si>
   <si>
     <t xml:space="preserve">etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geography</t>
   </si>
 </sst>
 </file>
@@ -135,7 +222,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,6 +243,24 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,7 +305,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -211,6 +316,22 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -230,10 +351,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F88" activeCellId="0" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1070,6 +1191,166 @@
         <v>26</v>
       </c>
     </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C81" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C82" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <f aca="false">AVERAGE(E82:G82)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <f aca="false">AVERAGE(E83:G83)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C84" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <f aca="false">AVERAGE(E84:G84)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C85" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <f aca="false">AVERAGE(E85:G85)</f>
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
finished map of list
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1315,10 +1315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1491,6 +1491,121 @@
       </c>
       <c r="J39" s="0" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various test cases #2
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">Geography</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">Test</t>
@@ -1317,8 +1323,8 @@
   </sheetPr>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1351,31 +1357,69 @@
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
@@ -1387,16 +1431,39 @@
       <c r="D15" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="I15" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="0" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
various test cases #4
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="position" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="e2Single" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="listBindTest" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -180,6 +181,15 @@
   </si>
   <si>
     <t xml:space="preserve">Test3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t3</t>
   </si>
 </sst>
 </file>
@@ -221,12 +231,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,6 +310,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,6 +327,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF4000"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -307,7 +397,7 @@
   </sheetPr>
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F88" activeCellId="0" sqref="F88"/>
     </sheetView>
   </sheetViews>
@@ -1323,8 +1413,8 @@
   </sheetPr>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1673,6 +1763,201 @@
       </c>
       <c r="H55" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various test cases #5
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="position" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="e2Single" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="listBindTest" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="e2Map" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="61">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -190,6 +191,21 @@
   </si>
   <si>
     <t xml:space="preserve">t3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
   </si>
 </sst>
 </file>
@@ -1783,7 +1799,7 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1969,4 +1985,71 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
various test cases #6
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -12,6 +12,7 @@
     <sheet name="e2Single" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="listBindTest" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="e2Map" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="e2MapBinds" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="65">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -206,6 +207,18 @@
   </si>
   <si>
     <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k</t>
   </si>
 </sst>
 </file>
@@ -247,12 +260,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -264,6 +283,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
         <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -301,7 +326,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -334,6 +359,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,7 +396,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -388,7 +421,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFBF00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF666699"/>
@@ -1429,8 +1462,8 @@
   </sheetPr>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G9" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1506,19 +1539,19 @@
       <c r="I13" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N13" s="0" t="s">
+      <c r="K13" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="O13" s="0" t="n">
+      <c r="O13" s="6" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1853,16 +1886,16 @@
       <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="n">
+      <c r="B6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="7" t="n">
         <v>16</v>
       </c>
       <c r="F6" s="0" t="n">
@@ -1873,16 +1906,16 @@
       <c r="A7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="n">
+      <c r="B7" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="7" t="n">
         <v>17</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -1893,14 +1926,14 @@
       <c r="A8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="n">
+      <c r="B8" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6" t="n">
+      <c r="D8" s="8"/>
+      <c r="E8" s="7" t="n">
         <v>18</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -1911,16 +1944,16 @@
       <c r="A9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="6" t="n">
+      <c r="C9" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
@@ -1929,16 +1962,16 @@
       <c r="A10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="6" t="n">
+      <c r="C10" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="7" t="n">
         <v>20</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -1992,10 +2025,369 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:D7"/>
+  <dimension ref="A2:K32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F28" s="9" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C29" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D29" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E29" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F29" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:I15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2004,43 +2396,139 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="B3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="G9" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="0" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="G11" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>60</v>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various test cases #7 & added freeze method for listOfMap
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="position" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="listBindTest" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="e2Map" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="e2MapBinds" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="mapList" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -260,7 +261,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,7 +289,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF8000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -326,7 +333,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,6 +371,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,7 +433,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFBF00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -446,7 +457,7 @@
   </sheetPr>
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F88" activeCellId="0" sqref="F88"/>
     </sheetView>
   </sheetViews>
@@ -2027,8 +2038,8 @@
   </sheetPr>
   <dimension ref="A2:K32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2387,7 +2398,7 @@
   <dimension ref="B3:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2529,6 +2540,127 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="n">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B4:F13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#4, #3] bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="position" sheetId="1" state="visible" r:id="rId2"/>
@@ -230,12 +230,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -264,6 +265,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -287,7 +295,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
     <fill>
@@ -337,7 +345,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,6 +374,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,10 +395,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,7 +461,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -1479,10 +1491,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1831,6 +1843,59 @@
       </c>
       <c r="H55" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7" t="n">
+        <v>43748</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="8"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="7" t="n">
+        <v>43748</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7" t="n">
+        <v>43752</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="7" t="n">
+        <v>43750</v>
       </c>
     </row>
   </sheetData>
@@ -1905,16 +1970,16 @@
       <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="n">
+      <c r="B6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="9" t="n">
         <v>16</v>
       </c>
       <c r="F6" s="0" t="n">
@@ -1925,16 +1990,16 @@
       <c r="A7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="n">
+      <c r="B7" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="9" t="n">
         <v>17</v>
       </c>
       <c r="F7" s="0" t="n">
@@ -1945,14 +2010,14 @@
       <c r="A8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="7" t="n">
+      <c r="B8" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7" t="n">
+      <c r="D8" s="10"/>
+      <c r="E8" s="9" t="n">
         <v>18</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -1963,16 +2028,16 @@
       <c r="A9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7" t="n">
+      <c r="B9" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
@@ -1981,16 +2046,16 @@
       <c r="A10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="9" t="n">
         <v>15</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="9" t="n">
         <v>20</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -2044,10 +2109,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K32"/>
+  <dimension ref="A2:K41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2073,7 +2138,7 @@
       <c r="A3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -2082,10 +2147,10 @@
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="n">
+      <c r="F3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2093,7 +2158,7 @@
       <c r="A4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2102,10 +2167,10 @@
       <c r="E4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7" t="n">
+      <c r="F4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2113,7 +2178,7 @@
       <c r="A5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="9" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -2122,10 +2187,10 @@
       <c r="E5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="7" t="n">
+      <c r="F5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2133,7 +2198,7 @@
       <c r="A6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -2142,10 +2207,10 @@
       <c r="E6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7" t="n">
+      <c r="F6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2153,7 +2218,7 @@
       <c r="A7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="9" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -2162,10 +2227,10 @@
       <c r="E7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7" t="n">
+      <c r="F7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2189,42 +2254,42 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2260,19 +2325,19 @@
       <c r="A20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B20" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D20" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E20" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F20" s="7" t="n">
+      <c r="B20" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G20" s="0" t="n">
@@ -2303,88 +2368,98 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="I23" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D28" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="E28" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F28" s="9" t="n">
+      <c r="B28" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F28" s="11" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9" t="n">
+      <c r="B29" s="11" t="n">
         <v>6</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="D29" s="9" t="n">
+      <c r="D29" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="E29" s="9" t="n">
+      <c r="E29" s="11" t="n">
         <v>9</v>
       </c>
-      <c r="F29" s="9" t="n">
+      <c r="F29" s="11" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="H31" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="H32" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I32" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J32" s="7" t="s">
+      <c r="J32" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="K32" s="9" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="n">
+        <v>43748</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7" t="n">
+        <v>43752</v>
       </c>
     </row>
   </sheetData>
@@ -2403,10 +2478,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:I15"/>
+  <dimension ref="A3:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2415,17 +2490,17 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="9" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G5" s="6" t="n">
@@ -2439,7 +2514,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="9" t="n">
         <v>4</v>
       </c>
       <c r="G6" s="6" t="n">
@@ -2453,7 +2528,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G7" s="6" t="n">
@@ -2478,7 +2553,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>56</v>
       </c>
       <c r="G9" s="6" t="n">
@@ -2492,12 +2567,12 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="6" t="n">
@@ -2509,7 +2584,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>59</v>
       </c>
       <c r="G12" s="6" t="n">
@@ -2521,7 +2596,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G13" s="6" t="n">
@@ -2548,6 +2623,16 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="n">
+        <v>43748</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
+        <v>43752</v>
       </c>
     </row>
   </sheetData>
@@ -2583,21 +2668,21 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="10" t="n">
+      <c r="B4" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="12" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10" t="n">
+      <c r="B5" s="12" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="n">
@@ -2611,7 +2696,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="10" t="n">
+      <c r="B6" s="12" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="6" t="n">
@@ -2625,7 +2710,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10" t="n">
+      <c r="B7" s="12" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="6" t="n">
@@ -2639,40 +2724,40 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F10" s="10" t="n">
+      <c r="B10" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="10" t="n">
+      <c r="B11" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="12" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="10" t="n">
+      <c r="B12" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" s="10" t="n">
+      <c r="B13" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2694,7 +2779,7 @@
   </sheetPr>
   <dimension ref="E2:K4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -2710,7 +2795,7 @@
       <c r="F2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -2730,7 +2815,7 @@
       <c r="F3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G3" s="11" t="n">
+      <c r="G3" s="0" t="n">
         <v>6</v>
       </c>
       <c r="I3" s="0" t="n">

</xml_diff>